<commit_message>
add GIT path on generating notebook part
</commit_message>
<xml_diff>
--- a/Generate_Deployment/Input_folder/PREPARE_ITEM_LIST_SI-0000_SR-00000_SR-00000_SYSTEM.xlsx
+++ b/Generate_Deployment/Input_folder/PREPARE_ITEM_LIST_SI-0000_SR-00000_SR-00000_SYSTEM.xlsx
@@ -1,33 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scb100690\Playground\test_repo\Generate_Deployment\Input_folder\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128B5D09-C3F3-486F-A33A-5A404A63859B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Howto" sheetId="1" r:id="rId1"/>
-    <sheet name="Config_List" sheetId="2" r:id="rId2"/>
-    <sheet name="U21_Import_ADF_Config" sheetId="3" r:id="rId3"/>
-    <sheet name="U22_Import_File_Config" sheetId="4" r:id="rId4"/>
-    <sheet name="U23_Import_Table_Definition" sheetId="5" r:id="rId5"/>
-    <sheet name="U24_Import_Interface_Mapping" sheetId="6" r:id="rId6"/>
-    <sheet name="99_Run_replace_DDL" sheetId="7" r:id="rId7"/>
-    <sheet name="ADB_Notebook_To_Shared_Folder" sheetId="8" r:id="rId8"/>
+    <sheet r:id="rId1" sheetId="1" name="Howto"/>
+    <sheet r:id="rId2" sheetId="2" name="Config_List"/>
+    <sheet r:id="rId3" sheetId="3" name="U21_Import_ADF_Config"/>
+    <sheet r:id="rId4" sheetId="4" name="U22_Import_File_Config"/>
+    <sheet r:id="rId5" sheetId="5" name="U23_Import_Table_Definition"/>
+    <sheet r:id="rId6" sheetId="6" name="U24_Import_Interface_Mapping"/>
+    <sheet r:id="rId7" sheetId="7" name="99_Run_replace_DDL"/>
+    <sheet r:id="rId8" sheetId="8" name="ADB_Notebook_To_Shared_Folder"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>SHARED_PATH</t>
   </si>
@@ -38,6 +32,9 @@
     <t>EXECUTE_FLAG</t>
   </si>
   <si>
+    <t>GIT_PATH</t>
+  </si>
+  <si>
     <t>/Shared/Execute/</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
     <t>/Shared/Utilities/U21_Import_ADF_Config</t>
   </si>
   <si>
+    <t>(ถ้าไม่มีแก้ไขใส่ 0 ที่ column GENERATE_FILE_FLAG)</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -200,6 +200,56 @@
     <t>/Shared/Utilities/U24_Import_Interface_Mapping_Config</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">ถ้าหากมี </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> แก้ไข view หรือ table ใส่ชื่อ view/table ที่ sheet 99_RUN_replace_DDL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ถ้าหากมี </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Notebook ที่ต้องการวางใน folder /Shared/ ที่ Databricks Please Fill sheet  ADB_Notebook_To_Shared_Folder</t>
+    </r>
+  </si>
+  <si>
     <t>Sheet</t>
   </si>
   <si>
@@ -218,7 +268,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -236,7 +286,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -253,7 +303,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -270,7 +320,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -279,9 +329,12 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
+      <t/>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -299,7 +352,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -343,7 +396,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -361,7 +414,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -375,7 +428,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFff0000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
@@ -430,10 +483,9 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
       </rPr>
       <t>/Shared/&lt;path&gt;/</t>
     </r>
@@ -442,13 +494,18 @@
     <t>The name of Notebook</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+    <t>1 for auto generate git folder with UR info, 0 for use like /Shared path</t>
+  </si>
+  <si>
+    <r>
+      <t/>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
       </rPr>
       <t>1</t>
     </r>
@@ -458,17 +515,15 @@
         <color rgb="FF000000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> if you want to execute it, </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
       </rPr>
       <t>0</t>
     </r>
@@ -478,70 +533,21 @@
         <color rgb="FF000000"/>
         <rFont val="Tahoma"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> if you don't</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ถ้าหากมี </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> แก้ไข view หรือ table ใส่ชื่อ view/table ที่ sheet 99_RUN_replace_DDL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ถ้าหากมี </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Notebook ที่ต้องการวางใน folder /Shared/ ที่ Databricks Please Fill sheet  ADB_Notebook_To_Shared_Folder</t>
-    </r>
-  </si>
-  <si>
-    <t>(ถ้าไม่มีแก้ไขใส่ 0 ที่ column GENERATE_FILE_FLAG)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -554,19 +560,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFC72E0F"/>
+      <color rgb="FFc72e0f"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFff0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -575,38 +581,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -619,87 +593,87 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEEBF7"/>
+        <fgColor rgb="FFdeebf7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE699"/>
+        <fgColor rgb="FFffe699"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
+        <fgColor rgb="FFe7e6e6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5B9BD5"/>
+        <fgColor rgb="FF5b9bd5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAFABAB"/>
+        <fgColor rgb="FFafabab"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
+        <fgColor rgb="FFe2f0d9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFff0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFBE5D6"/>
+        <fgColor rgb="FFfbe5d6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFffc000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDAE3F3"/>
+        <fgColor rgb="FFdae3f3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFffff00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
+        <fgColor rgb="FFfff2cc"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF92d050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDEDED"/>
+        <fgColor rgb="FFededed"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF00b050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6DCE5"/>
+        <fgColor rgb="FFd6dce5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF00b0f0"/>
       </patternFill>
     </fill>
   </fills>
@@ -713,16 +687,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,13 +733,13 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -780,7 +754,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -789,7 +763,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,123 +772,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -925,10 +906,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -966,71 +947,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1058,7 +1039,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1081,11 +1062,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1094,13 +1075,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1110,7 +1091,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1119,7 +1100,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1128,7 +1109,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1136,10 +1117,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1204,181 +1185,188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.25" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="38" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="119.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="24">
+      <c r="A1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+      <c r="A2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="26"/>
+      <c r="B10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="35" t="s">
+      <c r="B11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="A12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="36" t="s">
+      <c r="C12" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+      <c r="A14" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="36" t="s">
+      <c r="C14" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="35"/>
+      <c r="B15" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="36" t="s">
+      <c r="C15" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>79</v>
+      <c r="C17" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1387,171 +1375,172 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A14:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.75" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.75" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="38.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="48.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="13">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="13">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1559,77 +1548,77 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="30.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="32.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="24.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="8"/>
@@ -1640,7 +1629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1648,19 +1637,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="30.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1669,7 +1658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1677,58 +1666,58 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="22.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1737,7 +1726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1745,24 +1734,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="34.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1771,78 +1760,76 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="56.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1851,22 +1838,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="15.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1876,36 +1864,39 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{c799a265-e452-471a-9f71-28c814d4acbc}" enabled="1" method="Standard" siteId="{45202dee-4088-4e8c-8ebd-c01f56740e8f}" contentBits="0" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
modify input excel template
</commit_message>
<xml_diff>
--- a/Generate_Deployment/Input_folder/PREPARE_ITEM_LIST_SI-0000_SR-00000_SR-00000_SYSTEM.xlsx
+++ b/Generate_Deployment/Input_folder/PREPARE_ITEM_LIST_SI-0000_SR-00000_SR-00000_SYSTEM.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scb100690\Playground\EDW_UTILITIES\Generate_Deployment\Input_folder\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034753D8-113E-42DA-8C53-8A0B81B0BC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Howto"/>
-    <sheet r:id="rId2" sheetId="2" name="Config_List"/>
-    <sheet r:id="rId3" sheetId="3" name="U21_Import_ADF_Config"/>
-    <sheet r:id="rId4" sheetId="4" name="U22_Import_File_Config"/>
-    <sheet r:id="rId5" sheetId="5" name="U23_Import_Table_Definition"/>
-    <sheet r:id="rId6" sheetId="6" name="U24_Import_Interface_Mapping"/>
-    <sheet r:id="rId7" sheetId="7" name="99_Run_replace_DDL"/>
-    <sheet r:id="rId8" sheetId="8" name="ADB_Notebook_To_Shared_Folder"/>
+    <sheet name="Howto" sheetId="1" r:id="rId1"/>
+    <sheet name="Config_List" sheetId="2" r:id="rId2"/>
+    <sheet name="U21_Import_ADF_Config" sheetId="3" r:id="rId3"/>
+    <sheet name="U22_Import_File_Config" sheetId="4" r:id="rId4"/>
+    <sheet name="U23_Import_Table_Definition" sheetId="5" r:id="rId5"/>
+    <sheet name="U24_Import_Interface_Mapping" sheetId="6" r:id="rId6"/>
+    <sheet name="99_Run_replace_DDL" sheetId="7" r:id="rId7"/>
+    <sheet name="ADB_Notebook_To_Shared_Folder" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>SHARED_PATH</t>
   </si>
@@ -206,12 +212,322 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFff0000"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> แก้ไข view หรือ table ใส่ชื่อ view/table ที่ sheet 99_RUN_replace_DDL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ถ้าหากมี </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Notebook ที่ต้องการวางใน folder /Shared/ ที่ Databricks Please Fill sheet  ADB_Notebook_To_Shared_Folder</t>
+    </r>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Describ</t>
+  </si>
+  <si>
+    <t>Config_List</t>
+  </si>
+  <si>
+    <r>
+      <t>UR number like feature name if feature name is feature/jan2024_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>SI999-SR9999-SR9999_AML_ESL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> input like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>SI999-SR9999-SR9999_AML_ESL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mmmYYYY like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>jan2024</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">yyyy-mm-dd like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>2024-01-15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> on sheet that you want to generate or the sheet you edited and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> on the rest</t>
+    </r>
+  </si>
+  <si>
+    <t>System_name</t>
+  </si>
+  <si>
+    <t>Table name</t>
+  </si>
+  <si>
+    <t>Interface name</t>
+  </si>
+  <si>
+    <t>99_Run_replace_DDL</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Full Table name or View name that you edited like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">P1DSGEDW.SOME_TABLE_NAME </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> P1VSGEDW.SOME_TABLE_NAME</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">insert </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NEW </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>only for</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> new table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if the value of TABLE_OR_VIEW_LIST is the Existing Table, Existing View or New View Please Keep it </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <t>ADB_Notebook_To_Shared_Folder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Path of Shared folder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>/Shared/&lt;path&gt;/</t>
+    </r>
+  </si>
+  <si>
+    <t>The name of Notebook</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if you want to execute it, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if you don't</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
+      </rPr>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -219,24 +535,17 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> แก้ไข view หรือ table ใส่ชื่อ view/table ที่ sheet 99_RUN_replace_DDL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ถ้าหากมี </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
+      </rPr>
+      <t xml:space="preserve"> for auto generate git folder with UR info, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ถ้าไม่มีไม่ต้องใส่อะไร)</t>
+      </rPr>
+      <t>0</t>
     </r>
     <r>
       <rPr>
@@ -244,310 +553,101 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Notebook ที่ต้องการวางใน folder /Shared/ ที่ Databricks Please Fill sheet  ADB_Notebook_To_Shared_Folder</t>
-    </r>
-  </si>
-  <si>
-    <t>Sheet</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Describ</t>
-  </si>
-  <si>
-    <t>Config_List</t>
-  </si>
-  <si>
-    <r>
-      <t>UR number like feature name if feature name is feature/jan2024_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>SI999-SR9999-SR9999_AML_ESL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> input like </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>SI999-SR9999-SR9999_AML_ESL</t>
-    </r>
-  </si>
-  <si>
-    <t>MONTH_PERIOD_DEPLOY</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">mmmYYYY like </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>jan2024</t>
-    </r>
-  </si>
-  <si>
-    <t>DEPLOY_DATE</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">yyyy-mm-dd like </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>2024-01-15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> on sheet that you want to generate or the sheet you edited and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> on the rest</t>
-    </r>
-  </si>
-  <si>
-    <t>System_name</t>
-  </si>
-  <si>
-    <t>ADF_CONFIG file name with out file format</t>
-  </si>
-  <si>
-    <t>file_config file name with out file format</t>
-  </si>
-  <si>
-    <t>Schema name without 'P1'</t>
-  </si>
-  <si>
-    <t>Table name</t>
-  </si>
-  <si>
-    <t>Interface name</t>
-  </si>
-  <si>
-    <t>99_Run_replace_DDL</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Full Table name or View name that you edited like </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">P1DSGEDW.SOME_TABLE_NAME </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> P1VSGEDW.SOME_TABLE_NAME</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">insert </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">NEW </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>only for</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> new table</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> if the value of TABLE_OR_VIEW_LIST is the Existing Table, Existing View or New View Please Keep it </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>null</t>
-    </r>
-  </si>
-  <si>
-    <t>ADB_Notebook_To_Shared_Folder</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Path of Shared folder </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Shared/&lt;path&gt;/</t>
-    </r>
-  </si>
-  <si>
-    <t>The name of Notebook</t>
-  </si>
-  <si>
-    <t>1 for auto generate git folder with UR info, 0 for use like /Shared path</t>
-  </si>
-  <si>
-    <r>
-      <t/>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> if you want to execute it, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFff0000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> if you don't</t>
-    </r>
+      </rPr>
+      <t xml:space="preserve"> for use like /Shared path</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADF_CONFIG file name without file format </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LIST_JOB_SYSTEM_XXXXX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">file_config file name with out file format </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>REGISTER_CONFIG_SYSTEM_XXXXX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"FILE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Schema name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> without 'P1'</t>
+    </r>
+  </si>
+  <si>
+    <t>Information: UR_NO</t>
+  </si>
+  <si>
+    <t>Information: Email</t>
+  </si>
+  <si>
+    <t>Information: Month_Period</t>
+  </si>
+  <si>
+    <t>Information: Deploy_Date</t>
+  </si>
+  <si>
+    <t>your email use for jenkins parameters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -566,19 +666,45 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFc72e0f"/>
+      <color rgb="FFC72E0F"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -593,91 +719,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdeebf7"/>
+        <fgColor rgb="FFDEEBF7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffe699"/>
+        <fgColor rgb="FFFFE699"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFe7e6e6"/>
+        <fgColor rgb="FFE7E6E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5b9bd5"/>
+        <fgColor rgb="FF5B9BD5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFafabab"/>
+        <fgColor rgb="FFAFABAB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFe2f0d9"/>
+        <fgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFff0000"/>
+        <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfbe5d6"/>
+        <fgColor rgb="FFFBE5D6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffc000"/>
+        <fgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdae3f3"/>
+        <fgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfff2cc"/>
+        <fgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92d050"/>
+        <fgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFededed"/>
+        <fgColor rgb="FFEDEDED"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b050"/>
+        <fgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd6dce5"/>
+        <fgColor rgb="FFD6DCE5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b0f0"/>
+        <fgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -687,16 +813,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,13 +859,13 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -754,7 +880,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -763,8 +889,49 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -772,130 +939,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -906,10 +1072,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -947,71 +1113,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1039,7 +1205,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1062,11 +1228,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1075,13 +1241,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1091,7 +1257,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1100,7 +1266,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1109,7 +1275,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1117,10 +1283,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1185,22 +1351,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="38" width="29.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="119.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.25" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="24">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>61</v>
       </c>
@@ -1211,178 +1379,187 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>41</v>
+      <c r="B2" s="26" t="s">
+        <v>83</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="7" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="17" t="s">
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="7" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="21"/>
-      <c r="B7" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="7" t="s">
+    <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B13" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="7" t="s">
+    <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="26"/>
-      <c r="B10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="7" t="s">
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B15" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="29" t="s">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25"/>
+      <c r="B17" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="7" t="s">
+    <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="35"/>
-      <c r="B15" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="36"/>
-      <c r="B16" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1390,18 +1567,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="38.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="33.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="48.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.75" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.75" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
         <v>36</v>
@@ -1420,7 +1597,7 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>41</v>
       </c>
@@ -1443,7 +1620,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>46</v>
       </c>
@@ -1466,7 +1643,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>50</v>
       </c>
@@ -1489,7 +1666,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>54</v>
       </c>
@@ -1512,7 +1689,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1523,7 +1700,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1540,22 +1717,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="30.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="32.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="30.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1564,7 +1743,7 @@
       </c>
       <c r="C1" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -1573,52 +1752,52 @@
       </c>
       <c r="C2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="8"/>
@@ -1629,25 +1808,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="30.875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1658,7 +1839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1666,13 +1847,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="21.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1680,7 +1861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1688,7 +1869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1696,7 +1877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1704,7 +1885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1712,7 +1893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1726,7 +1907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1734,22 +1915,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="34.75" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1760,7 +1941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1768,13 +1949,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="56.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="56.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1782,7 +1963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1790,13 +1971,13 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1804,19 +1985,19 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1824,7 +2005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1838,7 +2019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1846,15 +2027,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +2049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1882,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1899,4 +2080,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c799a265-e452-471a-9f71-28c814d4acbc}" enabled="1" method="Standard" siteId="{45202dee-4088-4e8c-8ebd-c01f56740e8f}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>